<commit_message>
Excel de modelo de Dominio - Fabricante - Producto
</commit_message>
<xml_diff>
--- a/HojaVidaComputo/Accesorios - MuestreoDatos.xlsx
+++ b/HojaVidaComputo/Accesorios - MuestreoDatos.xlsx
@@ -5,20 +5,22 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://grchia-my.sharepoint.com/personal/jhonatan_gomez_wiga_io/Documents/Escritorio/UCO/DOO GIT/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://grchia-my.sharepoint.com/personal/jhonatan_gomez_wiga_io/Documents/Escritorio/UCO/DOO GIT/HojaVidaComputo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="64" documentId="8_{5F6CDBB6-63CB-49B4-BF45-CE4CAD9A884C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{777E991E-82EF-4139-94AA-5915F473DB96}"/>
+  <xr:revisionPtr revIDLastSave="66" documentId="8_{5F6CDBB6-63CB-49B4-BF45-CE4CAD9A884C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8C7CC10A-746F-4EF2-95FC-2B3912605E0E}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" firstSheet="1" activeTab="1" xr2:uid="{85AF6D48-FDD5-4A15-BC1B-8DA82DA63D0B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" firstSheet="1" activeTab="3" xr2:uid="{85AF6D48-FDD5-4A15-BC1B-8DA82DA63D0B}"/>
   </bookViews>
   <sheets>
     <sheet name="modelo de dominio anemico" sheetId="3" r:id="rId1"/>
     <sheet name="Objetos de dominio" sheetId="2" r:id="rId2"/>
     <sheet name="Accesorios" sheetId="1" r:id="rId3"/>
     <sheet name="AccesorioFabricante" sheetId="7" r:id="rId4"/>
-    <sheet name="Fabricante" sheetId="6" r:id="rId5"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId5"/>
+  </externalReferences>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -60,21 +62,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="15">
   <si>
     <t>Identificador</t>
   </si>
   <si>
     <t>Nombre</t>
-  </si>
-  <si>
-    <t>Lenovo</t>
-  </si>
-  <si>
-    <t>HP</t>
-  </si>
-  <si>
-    <t>Samsung</t>
   </si>
   <si>
     <t>Combinacion única</t>
@@ -120,7 +113,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -130,14 +123,6 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
@@ -193,19 +178,18 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -222,6 +206,26 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <xxl21:alternateUrls>
+      <xxl21:absoluteUrl r:id="rId2"/>
+    </xxl21:alternateUrls>
+    <sheetNames>
+      <sheetName val="Modelo de Dominio Anemico"/>
+      <sheetName val="Objetos de dominio"/>
+      <sheetName val="Fabricante"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1"/>
+      <sheetData sheetId="2"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
 </file>
 
 <file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
@@ -573,8 +577,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAB2B1D3-F4EF-49F9-AFA2-1ECC5999F861}">
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -586,44 +590,44 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>17</v>
+      <c r="A2" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>14</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" s="6" t="s">
+      <c r="A3" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="7" t="s">
-        <v>13</v>
-      </c>
       <c r="D3" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -660,8 +664,8 @@
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
-        <v>5</v>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -669,9 +673,9 @@
         <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C2" s="5" t="str">
+        <v>13</v>
+      </c>
+      <c r="C2" s="4" t="str">
         <f t="shared" ref="C2" si="0">B2</f>
         <v>Cargador</v>
       </c>
@@ -685,7 +689,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9B0AF81-F6C5-4CAD-AD40-930A9DE954FF}">
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
@@ -702,10 +706,10 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>5</v>
+        <v>6</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -713,15 +717,15 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C2" s="2" t="str">
-        <f>Fabricante!B2</f>
-        <v>Lenovo</v>
-      </c>
-      <c r="D2" s="5" t="str">
+        <v>13</v>
+      </c>
+      <c r="C2" s="2" t="e">
+        <f>#REF!</f>
+        <v>#REF!</v>
+      </c>
+      <c r="D2" s="4" t="e">
         <f>B2&amp;"-"&amp;C2</f>
-        <v>Cargador-Lenovo</v>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -729,82 +733,16 @@
         <v>1</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C3" s="2" t="str">
-        <f>Fabricante!B3</f>
-        <v>HP</v>
-      </c>
-      <c r="D3" s="5" t="str">
+        <v>13</v>
+      </c>
+      <c r="C3" s="2" t="e">
+        <f>#REF!</f>
+        <v>#REF!</v>
+      </c>
+      <c r="D3" s="4" t="e">
         <f>B3&amp;"-"&amp;C3</f>
-        <v>Cargador-HP</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00A79D92-EA4C-488F-8B64-F52D8425D357}">
-  <dimension ref="A1:D4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J16" sqref="J16"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="3" max="3" width="18.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="2">
-        <v>1</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" s="5" t="str">
-        <f>B2</f>
-        <v>Lenovo</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="2">
-        <v>2</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" s="5" t="str">
-        <f t="shared" ref="C3:C4" si="0">B3</f>
-        <v>HP</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="2">
-        <v>2</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>Samsung</v>
-      </c>
-      <c r="D4" s="3"/>
+        <v>#REF!</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>